<commit_message>
Presentielijst, Feedback en correcte instructie Opdracht 2
</commit_message>
<xml_diff>
--- a/Workshop/Deelnemerslijst 2017.xlsx
+++ b/Workshop/Deelnemerslijst 2017.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="43">
   <si>
     <t>Inventarisatie voor:</t>
   </si>
@@ -266,9 +266,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -295,6 +292,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,12 +644,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1040,7 +1040,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,163 +1051,187 @@
     <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="15"/>
+      <c r="C2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="16"/>
+      <c r="C3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="15"/>
+      <c r="C4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="15" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="15"/>
+      <c r="C6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="16"/>
+      <c r="C7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="15"/>
+      <c r="D8" s="18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="16"/>
+      <c r="C9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="15"/>
+      <c r="C10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="15"/>
+      <c r="C12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="17"/>
+      <c r="C13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>